<commit_message>
Add three new exercise - add clustered versions of the Sudoku solver
1. Add an Actor based Sudoku solver that sends itself sudoku problems
   over and over again in a loop
2. Add an Akka Cluster Client app to be used in step 3
3. Add an Akka Cluster Client Receptionist to the clustered solver
   and add a separate program that uses an Akka Cluster Client to
   send Sudoku problems to the clustered solver
</commit_message>
<xml_diff>
--- a/images/Raspberry PI Cluster with NeoPixel status indicator.xlsx
+++ b/images/Raspberry PI Cluster with NeoPixel status indicator.xlsx
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Raspberry PI 3 Model B (incl. shipping cost)</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/3055</t>
   </si>
   <si>
     <t>8 x WS2812 Led strip 5050 RGB</t>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>https://nl.aliexpress.com/item/8-channel-WS2812-5050-RGB-LED-lights-development-board-for-Arduino/32769045926.html?spm=a2g0s.9042311.0.0.Mwyjuo</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.de/Computer-met-n-board/RASPBERRY-PI-3/3/index.html?ACTION=3&amp;LA=446&amp;ARTICLE=164977&amp;GROUPID=8242&amp;artnr=RASPBERRY+PI+3&amp;SEARCH=raspberry%2Bpi%2B3&amp;trstct=pos_0</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:Z1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -660,14 +660,14 @@
       <c r="D4" s="6">
         <v>30.46</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>6</v>
+      <c r="E4" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
@@ -677,13 +677,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
@@ -696,7 +696,7 @@
     <row r="7" spans="1:26" ht="12">
       <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
@@ -706,14 +706,14 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="12">
       <c r="A8" s="11"/>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
@@ -728,7 +728,7 @@
     <row r="9" spans="1:26" ht="12">
       <c r="A9" s="11"/>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
@@ -738,14 +738,14 @@
         <v>2.75</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="12">
       <c r="A10" s="11"/>
       <c r="B10" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="14">
         <f>SUM(C4:C9)</f>
@@ -761,7 +761,7 @@
     <row r="11" spans="1:26" ht="12">
       <c r="A11" s="11"/>
       <c r="B11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="14">
         <f t="shared" ref="C11:D11" si="1">C10*$A$4</f>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="14">
         <f>D14*EuroToUSD</f>
@@ -804,16 +804,16 @@
         <v>25</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12">
       <c r="A15" s="11"/>
       <c r="B15" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="14">
         <f>D15*EuroToUSD</f>
@@ -823,13 +823,13 @@
         <v>0.95</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12">
       <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="14">
         <f>D16*EuroToUSD</f>
@@ -839,13 +839,13 @@
         <v>5.99</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12">
       <c r="A17" s="11"/>
       <c r="B17" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="14">
         <f t="shared" ref="C17:D17" si="2">SUM(C14:C16)</f>
@@ -860,7 +860,7 @@
     <row r="18" spans="1:5" ht="12">
       <c r="A18" s="11"/>
       <c r="B18" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="14">
         <f>C17*A14</f>
@@ -884,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="14">
         <f>D20*EuroToUSD</f>
@@ -894,13 +894,13 @@
         <v>9.9</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12">
       <c r="A21" s="4"/>
       <c r="B21" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="14">
         <f t="shared" ref="C21:D21" si="3">SUM(C20)</f>
@@ -914,7 +914,7 @@
     <row r="22" spans="1:5" ht="12">
       <c r="A22" s="4"/>
       <c r="B22" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="14">
         <f>C21*A20</f>
@@ -935,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="14">
         <f>D24*EuroToUSD</f>
@@ -945,13 +945,13 @@
         <v>15.41</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12">
       <c r="A25" s="4"/>
       <c r="B25" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="14">
         <f t="shared" ref="C25:D25" si="4">SUM(C24)</f>
@@ -965,7 +965,7 @@
     <row r="26" spans="1:5" ht="12">
       <c r="A26" s="4"/>
       <c r="B26" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="14">
         <f>C25*A24</f>
@@ -986,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="14">
         <f>D28*EuroToUSD</f>
@@ -996,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12">
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="14">
         <f>D30*EuroToUSD</f>
@@ -1019,13 +1019,13 @@
         <v>65</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12">
       <c r="A31" s="4"/>
       <c r="B31" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="14">
         <f t="shared" ref="C31:D31" si="5">SUM(C30)</f>
@@ -1039,7 +1039,7 @@
     <row r="32" spans="1:5" ht="12">
       <c r="A32" s="4"/>
       <c r="B32" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="14">
         <f>C31*A30</f>
@@ -1063,7 +1063,7 @@
     <row r="35" spans="1:4" ht="12">
       <c r="A35" s="4"/>
       <c r="B35" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="14">
         <f t="shared" ref="C35:D35" si="6">C32+C26+C22+C18+C11</f>

</xml_diff>

<commit_message>
Add three new exercise - add clustered versions of the Sudoku solver (#27)
1. Add an Actor based Sudoku solver that sends itself sudoku problems
   over and over again in a loop
2. Add an Akka Cluster Client app to be used in step 3
3. Add an Akka Cluster Client Receptionist to the clustered solver
   and add a separate program that uses an Akka Cluster Client to
   send Sudoku problems to the clustered solver
</commit_message>
<xml_diff>
--- a/images/Raspberry PI Cluster with NeoPixel status indicator.xlsx
+++ b/images/Raspberry PI Cluster with NeoPixel status indicator.xlsx
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Raspberry PI 3 Model B (incl. shipping cost)</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/3055</t>
   </si>
   <si>
     <t>8 x WS2812 Led strip 5050 RGB</t>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>https://nl.aliexpress.com/item/8-channel-WS2812-5050-RGB-LED-lights-development-board-for-Arduino/32769045926.html?spm=a2g0s.9042311.0.0.Mwyjuo</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.de/Computer-met-n-board/RASPBERRY-PI-3/3/index.html?ACTION=3&amp;LA=446&amp;ARTICLE=164977&amp;GROUPID=8242&amp;artnr=RASPBERRY+PI+3&amp;SEARCH=raspberry%2Bpi%2B3&amp;trstct=pos_0</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:Z1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -660,14 +660,14 @@
       <c r="D4" s="6">
         <v>30.46</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>6</v>
+      <c r="E4" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6">
         <f t="shared" si="0"/>
@@ -677,13 +677,13 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="12">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6">
         <f t="shared" si="0"/>
@@ -696,7 +696,7 @@
     <row r="7" spans="1:26" ht="12">
       <c r="A7" s="11"/>
       <c r="B7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="6">
         <f t="shared" si="0"/>
@@ -706,14 +706,14 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:26" ht="12">
       <c r="A8" s="11"/>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="6">
         <f t="shared" si="0"/>
@@ -728,7 +728,7 @@
     <row r="9" spans="1:26" ht="12">
       <c r="A9" s="11"/>
       <c r="B9" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="6">
         <f t="shared" si="0"/>
@@ -738,14 +738,14 @@
         <v>2.75</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:26" ht="12">
       <c r="A10" s="11"/>
       <c r="B10" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="14">
         <f>SUM(C4:C9)</f>
@@ -761,7 +761,7 @@
     <row r="11" spans="1:26" ht="12">
       <c r="A11" s="11"/>
       <c r="B11" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="14">
         <f t="shared" ref="C11:D11" si="1">C10*$A$4</f>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="14">
         <f>D14*EuroToUSD</f>
@@ -804,16 +804,16 @@
         <v>25</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="12">
       <c r="A15" s="11"/>
       <c r="B15" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="14">
         <f>D15*EuroToUSD</f>
@@ -823,13 +823,13 @@
         <v>0.95</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="12">
       <c r="A16" s="11"/>
       <c r="B16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="14">
         <f>D16*EuroToUSD</f>
@@ -839,13 +839,13 @@
         <v>5.99</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12">
       <c r="A17" s="11"/>
       <c r="B17" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="14">
         <f t="shared" ref="C17:D17" si="2">SUM(C14:C16)</f>
@@ -860,7 +860,7 @@
     <row r="18" spans="1:5" ht="12">
       <c r="A18" s="11"/>
       <c r="B18" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="14">
         <f>C17*A14</f>
@@ -884,7 +884,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20" s="14">
         <f>D20*EuroToUSD</f>
@@ -894,13 +894,13 @@
         <v>9.9</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12">
       <c r="A21" s="4"/>
       <c r="B21" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C21" s="14">
         <f t="shared" ref="C21:D21" si="3">SUM(C20)</f>
@@ -914,7 +914,7 @@
     <row r="22" spans="1:5" ht="12">
       <c r="A22" s="4"/>
       <c r="B22" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="14">
         <f>C21*A20</f>
@@ -935,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="14">
         <f>D24*EuroToUSD</f>
@@ -945,13 +945,13 @@
         <v>15.41</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="12">
       <c r="A25" s="4"/>
       <c r="B25" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="14">
         <f t="shared" ref="C25:D25" si="4">SUM(C24)</f>
@@ -965,7 +965,7 @@
     <row r="26" spans="1:5" ht="12">
       <c r="A26" s="4"/>
       <c r="B26" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26" s="14">
         <f>C25*A24</f>
@@ -986,7 +986,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C28" s="14">
         <f>D28*EuroToUSD</f>
@@ -996,7 +996,7 @@
         <v>3</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="12">
@@ -1009,7 +1009,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" s="14">
         <f>D30*EuroToUSD</f>
@@ -1019,13 +1019,13 @@
         <v>65</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12">
       <c r="A31" s="4"/>
       <c r="B31" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C31" s="14">
         <f t="shared" ref="C31:D31" si="5">SUM(C30)</f>
@@ -1039,7 +1039,7 @@
     <row r="32" spans="1:5" ht="12">
       <c r="A32" s="4"/>
       <c r="B32" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C32" s="14">
         <f>C31*A30</f>
@@ -1063,7 +1063,7 @@
     <row r="35" spans="1:4" ht="12">
       <c r="A35" s="4"/>
       <c r="B35" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="14">
         <f t="shared" ref="C35:D35" si="6">C32+C26+C22+C18+C11</f>

</xml_diff>